<commit_message>
Move island consts. closer
Orkney and Na h'... are closer to main island
</commit_message>
<xml_diff>
--- a/UK_block_map.xlsx
+++ b/UK_block_map.xlsx
@@ -26,7 +26,7 @@
     <author>Mike Guidry</author>
   </authors>
   <commentList>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="U6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -25132,10 +25132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK60"/>
+  <dimension ref="A6:AMK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25144,12 +25144,12 @@
     <col min="37" max="1025" width="10.5546875" style="593" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="U1" s="592" t="s">
+    <row r="6" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="U6" s="592" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:22" x14ac:dyDescent="0.3">
       <c r="M10" s="1" t="s">
         <v>1</v>
       </c>
@@ -25169,8 +25169,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C11" s="632" t="s">
+    <row r="11" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F11" s="632" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="7" t="s">
@@ -25192,7 +25192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:22" x14ac:dyDescent="0.3">
       <c r="L12" s="13" t="s">
         <v>14</v>
       </c>
@@ -25209,7 +25209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:22" x14ac:dyDescent="0.3">
       <c r="L13" s="18" t="s">
         <v>19</v>
       </c>
@@ -25223,7 +25223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:22" x14ac:dyDescent="0.3">
       <c r="K14" s="22" t="s">
         <v>23</v>
       </c>
@@ -25240,7 +25240,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:22" x14ac:dyDescent="0.3">
       <c r="J15" s="27" t="s">
         <v>28</v>
       </c>
@@ -25275,7 +25275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:22" x14ac:dyDescent="0.3">
       <c r="J16" s="37" t="s">
         <v>39</v>
       </c>

</xml_diff>